<commit_message>
CPMV parameters when mismatch
</commit_message>
<xml_diff>
--- a/AMC_examples_data/AMC_examples_data_ex3.xlsx
+++ b/AMC_examples_data/AMC_examples_data_ex3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\AMC_examples_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8DF462-2272-41AD-B71B-C0E1EF84F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116B27B0-A1A1-4CA8-9486-6CB4B1EBD6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
+    <workbookView xWindow="2895" yWindow="1695" windowWidth="18030" windowHeight="11415" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>frame_h</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>VQ_best</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F28914-79CE-4C5A-92B2-E41C9BEF8F7E}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:S3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -519,8 +522,11 @@
       <c r="S1" t="s">
         <v>17</v>
       </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -578,8 +584,11 @@
       <c r="S2">
         <v>0</v>
       </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -605,17 +614,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>